<commit_message>
modify document about linux device model
</commit_message>
<xml_diff>
--- a/Linux/DeviceDrivers/Document/0.Linux设备模型_结构体_函数.xlsx
+++ b/Linux/DeviceDrivers/Document/0.Linux设备模型_结构体_函数.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FD59E13D-E9DE-45F2-9712-34B03CB9647A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Linux设备模型" sheetId="1" r:id="rId1"/>
     <sheet name="kobject_add" sheetId="2" r:id="rId2"/>
     <sheet name="sysfs" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="239">
   <si>
     <t>kobject</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -776,44 +775,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">fs/sysfs/mount.c
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>内部数据和函数</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>:
-static struct kernfs_root *sysfs_root;
-struct kernfs_node *sysfs_root_kn;
-static struct file_system_type sysfs_fs_type = {
-    .name     = "sysfs",
-    .mount    = sysfs_mount,
-    .kill_sb  = sysfs_kill_sb,
-    .fs_flags = FS_USERNS_VISIBLE | FS_USERNS_MOUNT,
-};
-int __init sysfs_init(void);
-static struct dentry *sysfs_mount(
-        struct file_system_type *fs_type, int flags, const char *dev_name, void *data);
-static void sysfs_kill_sb(struct super_block *sb);</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>include/linux/fs.h
 struct inode_operations {
     struct dentry * (*lookup) (struct inode *,struct dentry *, unsigned int);
@@ -1558,15 +1519,6 @@
   </si>
   <si>
     <t>fs-sysfs-file</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fs/sysfs/file.c
-EXPORT_SYMBOL_GPL:
-int sysfs_create_file_ns(struct kobject *kobj, const struct attribute *attr,
-        const void *ns);
-void sysfs_remove_file_ns(struct kobject *kobj, const struct attribute *attr,
-        const void *ns);</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2771,12 +2723,241 @@
     <t xml:space="preserve">    .show  = kobj_attr_show,</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>fs-sysfs-group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fs-sysfs-symlink</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fs/sysfs/file.c
+EXPORT_SYMBOL_GPL:
+int sysfs_create_file_ns(struct kobject *kobj, const struct attribute *attr,
+        const void *ns);
+int sysfs_create_files(struct kobject *kobj, const struct attribute **ptr);
+int sysfs_add_file_to_group(struct kobject *kobj, const struct attribute *attr,
+        const char *group);
+void sysfs_remove_file_ns(struct kobject *kobj, const struct attribute *attr,
+        const void *ns);
+void sysfs_remove_files(struct kobject *kobj, const struct attribute **ptr);
+void sysfs_remove_file_from_group(struct kobject *kobj, const struct attribute *attr,
+        const char *group);
+int sysfs_create_bin_file(struct kobject *kobj, const struct bin_attribute *attr);
+void sysfs_remove_bin_file(struct kobject *kobj, const struct bin_attribute *attr);
+void sysfs_notify(struct kobject *kobj, const char *dir, const char *attr);
+int sysfs_chmod_file(struct kobject *kobj, const struct attribute *attr, umode_t mode);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fs/sysfs/group.c
+EXPORT_SYMBOL_GPL:
+int sysfs_create_group(struct kobject *kobj, const struct attribute_group *grp);
+int sysfs_create_groups(struct kobject *kobj, const struct attribute_group **groups);
+int sysfs_update_group(struct kobject *kobj, const struct attribute_group *grp);
+void sysfs_remove_group(struct kobject *kobj, const struct attribute_group *grp);
+void sysfs_remove_groups(struct kobject *kobj, const struct attribute_group **groups);
+int sysfs_merge_group(struct kobject *kobj, const struct attribute_group *grp);
+void sysfs_unmerge_group(struct kobject *kobj, const struct attribute_group *grp);
+int sysfs_add_link_to_group(struct kobject *kobj, const char *group_name,
+        struct kobject *target, const char *link_name);
+void sysfs_remove_link_from_group(struct kobject *kobj, const char *group_name,
+        const char *link_name);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">fs/sysfs/mount.c
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>无</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">EXPORT_SYMBOL_GPL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>内部数据和函数</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>:
+static struct kernfs_root *sysfs_root;
+struct kernfs_node *sysfs_root_kn;
+static struct file_system_type sysfs_fs_type = {
+    .name     = "sysfs",
+    .mount    = sysfs_mount,
+    .kill_sb  = sysfs_kill_sb,
+    .fs_flags = FS_USERNS_VISIBLE | FS_USERNS_MOUNT,
+};
+int __init sysfs_init(void);
+static struct dentry *sysfs_mount(
+        struct file_system_type *fs_type, int flags, const char *dev_name, void *data);
+static void sysfs_kill_sb(struct super_block *sb);</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fs/sysfs/symlink.c
+EXPORT_SYMBOL_GPL:
+int sysfs_create_link(struct kobject *kobj, struct kobject *target, const char *name);
+void sysfs_remove_link(struct kobject *kobj, const char *name);
+int sysfs_rename_link_ns(struct kobject *kobj, struct kobject *targ,
+        const char *old, const char *new, const void *new_ns);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attribute_group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>include/linux/sysfs.h
+struct attribute_group {
+    const char           *name;
+    umode_t              (*is_visible)(struct kobject *, struct attribute *, int);
+    struct attribute     **attrs;
+    struct bin_attribute **bin_attrs;
+};</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kobj_attribute</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">include/linux/kobject.h
+struct kobj_attribute {
+    struct attribute attr;
+    ssize_t (*show)(struct kobject *kobj, struct kobj_attribute *attr,
+            char *buf);
+    ssize_t (*store)(struct kobject *kobj, struct kobj_attribute *attr,
+            const char *buf, size_t count);
+};
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>注</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>:
+show</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>函数</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>和</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> store</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>函数</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>需要自己实现</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2927,7 +3108,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -2962,7 +3143,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -3139,21 +3320,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="2.625" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.875" style="1" bestFit="1" customWidth="1"/>
@@ -3162,12 +3343,12 @@
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:4">
       <c r="B1" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4">
       <c r="B2" s="5" t="s">
         <v>57</v>
       </c>
@@ -3178,7 +3359,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" ht="48">
       <c r="B3" s="2" t="s">
         <v>54</v>
       </c>
@@ -3187,7 +3368,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="2:4" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" ht="409.5">
       <c r="B4" s="2" t="s">
         <v>64</v>
       </c>
@@ -3196,7 +3377,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="2:4" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" ht="409.5">
       <c r="B5" s="2" t="s">
         <v>66</v>
       </c>
@@ -3205,47 +3386,47 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="2:4" ht="384" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4" ht="384">
       <c r="B6" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="2:4" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" ht="409.5">
       <c r="B7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="336">
+      <c r="B8" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="336" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="108" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="108">
       <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="2:4" ht="348" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:4" ht="348">
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
@@ -3253,10 +3434,10 @@
         <v>6</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="144" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="144">
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -3264,30 +3445,30 @@
         <v>12</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="409.5" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="409.5">
       <c r="B12" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="48" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="48">
       <c r="B13" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="120" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="120">
       <c r="B14" s="2" t="s">
         <v>59</v>
       </c>
@@ -3296,7 +3477,7 @@
       </c>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="2:4" ht="144" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:4" ht="144">
       <c r="B15" s="2" t="s">
         <v>61</v>
       </c>
@@ -3305,122 +3486,158 @@
       </c>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="2:4" ht="72" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:4" ht="84">
       <c r="B16" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="2:4" ht="72">
+      <c r="B17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="84" x14ac:dyDescent="0.2">
-      <c r="B17" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="2:4" ht="96" x14ac:dyDescent="0.2">
+      <c r="D17" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="84">
       <c r="B18" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="2:4" ht="96">
+      <c r="B19" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="72" x14ac:dyDescent="0.2">
-      <c r="B19" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="180" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="192">
       <c r="B20" s="2" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="336" x14ac:dyDescent="0.2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="156">
       <c r="B21" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="192">
+      <c r="B22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="72">
+      <c r="B23" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="132">
+      <c r="B24" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="2:4" ht="336">
+      <c r="B25" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="240" x14ac:dyDescent="0.2">
-      <c r="B22" s="2" t="s">
+      <c r="D25" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="240">
+      <c r="B26" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D26" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="228">
+      <c r="B27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="84">
+      <c r="B28" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" ht="228" x14ac:dyDescent="0.2">
-      <c r="B23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" ht="84" x14ac:dyDescent="0.2">
-      <c r="B24" s="2" t="s">
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="2:4" ht="96">
+      <c r="B29" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="2:4" ht="96" x14ac:dyDescent="0.2">
-      <c r="B25" s="2" t="s">
+      <c r="C29" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="2:4" ht="120">
+      <c r="B30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="72">
+      <c r="B31" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="2:4" ht="120" x14ac:dyDescent="0.2">
-      <c r="B26" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" ht="72" x14ac:dyDescent="0.2">
-      <c r="B27" s="2" t="s">
+      <c r="C31" s="3"/>
+      <c r="D31" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -3431,19 +3648,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{609B74B3-0665-44FD-8CC1-2753055AA699}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AH31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="16384" width="2.625" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:34">
       <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
@@ -3451,7 +3668,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:34">
       <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
@@ -3459,7 +3676,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:34">
       <c r="D4" s="4" t="s">
         <v>15</v>
       </c>
@@ -3467,7 +3684,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:34">
       <c r="D5" s="4" t="s">
         <v>16</v>
       </c>
@@ -3475,7 +3692,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:34">
       <c r="E6" s="4" t="s">
         <v>17</v>
       </c>
@@ -3483,7 +3700,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:34">
       <c r="E7" s="4" t="s">
         <v>20</v>
       </c>
@@ -3491,7 +3708,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:34">
       <c r="E8" s="4" t="s">
         <v>21</v>
       </c>
@@ -3499,7 +3716,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:34">
       <c r="F9" s="4" t="s">
         <v>22</v>
       </c>
@@ -3507,7 +3724,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:34">
       <c r="G10" s="4" t="s">
         <v>23</v>
       </c>
@@ -3515,7 +3732,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:34">
       <c r="H11" s="4" t="s">
         <v>24</v>
       </c>
@@ -3523,7 +3740,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:34">
       <c r="F12" s="4" t="s">
         <v>25</v>
       </c>
@@ -3531,7 +3748,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:34">
       <c r="G13" s="4" t="s">
         <v>33</v>
       </c>
@@ -3539,7 +3756,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:34">
       <c r="H14" s="4" t="s">
         <v>35</v>
       </c>
@@ -3547,7 +3764,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:34">
       <c r="I15" s="4" t="s">
         <v>37</v>
       </c>
@@ -3555,7 +3772,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:34">
       <c r="I16" s="4" t="s">
         <v>38</v>
       </c>
@@ -3563,7 +3780,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="6:34" x14ac:dyDescent="0.2">
+    <row r="17" spans="6:34">
       <c r="H17" s="4" t="s">
         <v>36</v>
       </c>
@@ -3571,7 +3788,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="6:34" x14ac:dyDescent="0.2">
+    <row r="18" spans="6:34">
       <c r="I18" s="4" t="s">
         <v>39</v>
       </c>
@@ -3579,7 +3796,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="6:34" x14ac:dyDescent="0.2">
+    <row r="19" spans="6:34">
       <c r="I19" s="4" t="s">
         <v>40</v>
       </c>
@@ -3587,7 +3804,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="6:34" x14ac:dyDescent="0.2">
+    <row r="20" spans="6:34">
       <c r="I20" s="4" t="s">
         <v>41</v>
       </c>
@@ -3595,7 +3812,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="6:34" x14ac:dyDescent="0.2">
+    <row r="21" spans="6:34">
       <c r="F21" s="4" t="s">
         <v>26</v>
       </c>
@@ -3603,7 +3820,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="6:34" x14ac:dyDescent="0.2">
+    <row r="22" spans="6:34">
       <c r="G22" s="4" t="s">
         <v>42</v>
       </c>
@@ -3611,7 +3828,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="6:34" x14ac:dyDescent="0.2">
+    <row r="23" spans="6:34">
       <c r="H23" s="4" t="s">
         <v>44</v>
       </c>
@@ -3619,7 +3836,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="6:34" x14ac:dyDescent="0.2">
+    <row r="24" spans="6:34">
       <c r="I24" s="4" t="s">
         <v>45</v>
       </c>
@@ -3627,7 +3844,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="6:34" x14ac:dyDescent="0.2">
+    <row r="25" spans="6:34">
       <c r="J25" s="4" t="s">
         <v>46</v>
       </c>
@@ -3635,7 +3852,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="6:34" x14ac:dyDescent="0.2">
+    <row r="26" spans="6:34">
       <c r="F26" s="4" t="s">
         <v>27</v>
       </c>
@@ -3643,7 +3860,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="6:34" x14ac:dyDescent="0.2">
+    <row r="27" spans="6:34">
       <c r="G27" s="4" t="s">
         <v>49</v>
       </c>
@@ -3651,7 +3868,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="6:34" x14ac:dyDescent="0.2">
+    <row r="28" spans="6:34">
       <c r="F28" s="4" t="s">
         <v>24</v>
       </c>
@@ -3659,7 +3876,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="6:34" x14ac:dyDescent="0.2">
+    <row r="29" spans="6:34">
       <c r="F29" s="4" t="s">
         <v>28</v>
       </c>
@@ -3667,7 +3884,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="6:34" x14ac:dyDescent="0.2">
+    <row r="30" spans="6:34">
       <c r="F30" s="4" t="s">
         <v>29</v>
       </c>
@@ -3675,7 +3892,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="6:34" x14ac:dyDescent="0.2">
+    <row r="31" spans="6:34">
       <c r="G31" s="4" t="s">
         <v>51</v>
       </c>
@@ -3690,299 +3907,299 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78FF0051-E4FF-4B66-949D-B8AE3CE16B24}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AH127"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="AV69" sqref="AV69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="16384" width="2.625" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:34">
       <c r="B2" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="3" spans="2:34" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="2:34">
       <c r="B3" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH3" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="2:34">
+      <c r="C4" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="AH3" s="4" t="s">
+      <c r="AH4" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="C4" s="4" t="s">
+    <row r="5" spans="2:34">
+      <c r="D5" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="AH4" s="4" t="s">
+      <c r="AH5" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="D5" s="4" t="s">
+    <row r="6" spans="2:34">
+      <c r="E6" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="AH5" s="4" t="s">
+      <c r="AH6" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="2:34">
+      <c r="F7" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="6" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="E6" s="4" t="s">
+      <c r="AH7" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="2:34">
+      <c r="G8" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="AH6" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="F7" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH7" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="G8" s="4" t="s">
-        <v>121</v>
       </c>
       <c r="AH8" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:34">
       <c r="G9" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="AH9" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="2:34">
+      <c r="B11" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="AH11" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="2:34">
+      <c r="B12" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="2:34">
+      <c r="B13" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="2:34">
+      <c r="B14" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="2:34">
+      <c r="B15" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="2:34">
+      <c r="B16" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="2:34">
+      <c r="B18" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="2:34">
+      <c r="B19" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="2:34">
+      <c r="B20" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="AH9" s="4" t="s">
+      <c r="AH20" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="2:34">
+      <c r="C21" s="4" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="11" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B11" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="AH11" s="4" t="s">
+      <c r="AH21" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="2:34">
+      <c r="D22" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="AH22" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="2:34">
+      <c r="E23" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH23" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="2:34">
+      <c r="F24" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="AH24" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="2:34">
+      <c r="G25" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="AH25" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="2:34">
+      <c r="H26" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH26" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="2:34">
+      <c r="I27" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH27" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B12" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="13" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B13" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="14" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B14" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="15" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B15" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B16" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B18" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="19" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B19" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="20" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B20" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="AH20" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="C21" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="AH21" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="22" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="D22" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="AH22" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="E23" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="AH23" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="F24" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="AH24" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="25" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="G25" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="AH25" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="H26" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="AH26" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="I27" s="4" t="s">
+    <row r="28" spans="2:34">
+      <c r="J28" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="AH27" s="4" t="s">
+      <c r="AH28" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="2:34">
+      <c r="K29" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="28" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="J28" s="4" t="s">
+      <c r="AH29" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="AH28" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="29" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="K29" s="4" t="s">
+    </row>
+    <row r="30" spans="2:34">
+      <c r="L30" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="AH29" s="4" t="s">
+      <c r="AH30" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="L30" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH30" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="31" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:34">
       <c r="M31" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="33" spans="2:34" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="33" spans="2:34">
       <c r="B33" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AH33" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:34">
       <c r="B34" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="2:34">
+      <c r="B35" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="2:34">
+      <c r="B36" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B35" s="4" t="s">
+    <row r="37" spans="2:34">
+      <c r="B37" s="4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B36" s="4" t="s">
+    <row r="38" spans="2:34">
+      <c r="B38" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="37" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B37" s="4" t="s">
+    <row r="39" spans="2:34">
+      <c r="B39" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="38" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B38" s="4" t="s">
+    <row r="40" spans="2:34">
+      <c r="B40" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="39" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B39" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="40" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B40" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="41" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:34">
       <c r="B41" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="43" spans="2:34" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="2:34">
       <c r="B43" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="44" spans="2:34">
+      <c r="B44" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="45" spans="2:34">
+      <c r="C45" s="4" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="44" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B44" s="4" t="s">
+    <row r="46" spans="2:34">
+      <c r="D46" s="4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="45" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="C45" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="46" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="D46" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="47" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:34">
       <c r="C47" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:34">
       <c r="D48" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="5:34" x14ac:dyDescent="0.2">
+    <row r="49" spans="5:34">
       <c r="E49" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="5:34" x14ac:dyDescent="0.2">
+    <row r="50" spans="5:34">
       <c r="F50" s="4" t="s">
         <v>21</v>
       </c>
@@ -3990,7 +4207,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="5:34" x14ac:dyDescent="0.2">
+    <row r="51" spans="5:34">
       <c r="G51" s="4" t="s">
         <v>25</v>
       </c>
@@ -3998,7 +4215,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="5:34" x14ac:dyDescent="0.2">
+    <row r="52" spans="5:34">
       <c r="H52" s="4" t="s">
         <v>33</v>
       </c>
@@ -4006,23 +4223,23 @@
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="5:34" x14ac:dyDescent="0.2">
+    <row r="53" spans="5:34">
       <c r="I53" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="AH53" s="7" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="54" spans="5:34" x14ac:dyDescent="0.2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="54" spans="5:34">
       <c r="H54" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="AH54" s="7" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="55" spans="5:34" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="55" spans="5:34">
       <c r="G55" s="4" t="s">
         <v>26</v>
       </c>
@@ -4030,7 +4247,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="5:34" x14ac:dyDescent="0.2">
+    <row r="56" spans="5:34">
       <c r="H56" s="4" t="s">
         <v>42</v>
       </c>
@@ -4038,7 +4255,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="5:34" x14ac:dyDescent="0.2">
+    <row r="57" spans="5:34">
       <c r="I57" s="4" t="s">
         <v>44</v>
       </c>
@@ -4046,23 +4263,23 @@
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="5:34" x14ac:dyDescent="0.2">
+    <row r="58" spans="5:34">
       <c r="J58" s="4" t="s">
         <v>45</v>
       </c>
       <c r="AH58" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="59" spans="5:34" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" spans="5:34">
       <c r="K59" s="4" t="s">
         <v>46</v>
       </c>
       <c r="AH59" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="60" spans="5:34" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="5:34">
       <c r="L60" s="4" t="s">
         <v>35</v>
       </c>
@@ -4070,433 +4287,433 @@
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="5:34" x14ac:dyDescent="0.2">
+    <row r="61" spans="5:34">
       <c r="M61" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="AH61" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="62" spans="5:34">
+      <c r="L62" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="AH62" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="63" spans="5:34">
+      <c r="L63" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="AH63" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="AH61" s="4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="62" spans="5:34" x14ac:dyDescent="0.2">
-      <c r="L62" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="AH62" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="63" spans="5:34" x14ac:dyDescent="0.2">
-      <c r="L63" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="AH63" s="7" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="64" spans="5:34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="5:34">
       <c r="L64" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AH64" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="66" spans="2:34" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="66" spans="2:34">
       <c r="B66" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="AH66" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="67" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:34">
       <c r="B67" s="4" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="68" spans="2:34" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="68" spans="2:34">
       <c r="B68" s="4" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="69" spans="2:34" x14ac:dyDescent="0.2">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="69" spans="2:34">
       <c r="B69" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="71" spans="2:34" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="71" spans="2:34">
       <c r="B71" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="AH71" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:34">
       <c r="B72" s="4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="73" spans="2:34" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="73" spans="2:34">
       <c r="B73" s="4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="74" spans="2:34" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="74" spans="2:34">
       <c r="B74" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="76" spans="2:34" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="76" spans="2:34">
       <c r="B76" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="AH76" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="77" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:34">
       <c r="B77" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="78" spans="2:34" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="78" spans="2:34">
       <c r="B78" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="79" spans="2:34" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="79" spans="2:34">
       <c r="B79" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="81" spans="2:34">
+      <c r="B81" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="82" spans="2:34">
+      <c r="B82" s="4" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="81" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B81" s="4" t="s">
+      <c r="AH82" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="82" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B82" s="4" t="s">
+    <row r="83" spans="2:34">
+      <c r="C83" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="AH82" s="4" t="s">
+      <c r="AH83" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="84" spans="2:34">
+      <c r="D84" s="4" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="83" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="C83" s="4" t="s">
+      <c r="AH84" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="85" spans="2:34">
+      <c r="E85" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="AH83" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="84" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="D84" s="4" t="s">
+      <c r="AH85" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="86" spans="2:34">
+      <c r="F86" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="AH84" s="4" t="s">
+      <c r="AH86" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="87" spans="2:34">
+      <c r="G87" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="AH87" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="88" spans="2:34">
+      <c r="H88" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="85" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="E85" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AH85" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="86" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="F86" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="AH86" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="87" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="G87" s="4" t="s">
+      <c r="AH88" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="89" spans="2:34">
+      <c r="I89" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="AH87" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="88" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="H88" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="AH88" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="89" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="I89" s="4" t="s">
-        <v>147</v>
-      </c>
       <c r="AH89" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="90" spans="2:34" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="90" spans="2:34">
       <c r="I90" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="AH90" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="91" spans="2:34" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="91" spans="2:34">
       <c r="J91" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AH91" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="92" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:34">
       <c r="J92" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AH92" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="93" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:34">
       <c r="J93" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AH93" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="94" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:34">
       <c r="J94" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH94" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="AH94" s="4" t="s">
+    </row>
+    <row r="95" spans="2:34">
+      <c r="K95" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="AH95" s="4" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="95" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="K95" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="AH95" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="96" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:34">
       <c r="K96" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="AH96" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="97" spans="2:34" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="97" spans="2:34">
       <c r="J97" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AH97" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="99" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:34">
       <c r="B99" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="AH99" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="100" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:34">
       <c r="B100" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="101" spans="2:34" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="101" spans="2:34">
       <c r="B101" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="102" spans="2:34">
+      <c r="B102" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="103" spans="2:34">
+      <c r="B103" s="4" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="102" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B102" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="103" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B103" s="4" t="s">
+    <row r="104" spans="2:34">
+      <c r="B104" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="106" spans="2:34">
+      <c r="B106" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="107" spans="2:34">
+      <c r="B107" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="AH107" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="108" spans="2:34">
+      <c r="C108" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="AH108" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="109" spans="2:34">
+      <c r="D109" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="AH109" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="110" spans="2:34">
+      <c r="E110" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="AH110" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="111" spans="2:34">
+      <c r="F111" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="AH111" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="112" spans="2:34">
+      <c r="G112" s="4" t="s">
         <v>186</v>
-      </c>
-    </row>
-    <row r="104" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B104" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="106" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B106" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="107" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B107" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="AH107" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="108" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="C108" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="AH108" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="109" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="D109" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="AH109" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="110" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="E110" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="AH110" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="111" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="F111" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="AH111" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="112" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="G112" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="AH112" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="113" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:34">
       <c r="G113" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="AH113" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="114" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:34">
       <c r="H114" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="AH114" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="115" spans="2:34" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="115" spans="2:34">
       <c r="I115" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="AH115" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="116" spans="2:34" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="116" spans="2:34">
       <c r="J116" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="AH116" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="AH116" s="8" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="117" spans="2:34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="117" spans="2:34">
       <c r="G117" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AH117" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="118" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:34">
       <c r="G118" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AH118" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="120" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:34">
       <c r="B120" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="121" spans="2:34">
+      <c r="B121" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="AH121" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="122" spans="2:34">
+      <c r="C122" s="4" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="121" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B121" s="4" t="s">
+      <c r="AH122" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="123" spans="2:34">
+      <c r="D123" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="AH121" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="122" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="C122" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="AH122" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="123" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="D123" s="4" t="s">
+      <c r="AH123" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="124" spans="2:34">
+      <c r="E124" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="AH124" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="125" spans="2:34">
+      <c r="F125" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="AH123" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="124" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="E124" s="4" t="s">
+      <c r="AH125" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="AH124" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="125" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="F125" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="AH125" s="4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="126" spans="2:34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="126" spans="2:34">
       <c r="G126" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AH126" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="127" spans="2:34">
+      <c r="H127" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="AH126" s="4" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="127" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="H127" s="4" t="s">
-        <v>226</v>
-      </c>
       <c r="AH127" s="8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>